<commit_message>
Final submission: Excel-driven Playwright tests with comprehensive documentation
- Updated README.md with complete setup and usage instructions
- Fixed test file to properly detect output textarea
- All 41 tests passing (25 positive + 15 negative + 1 load test)
- Screenshots properly labeled (PASS/NEG/EMPTY/NO_OUTPUT)
- Excel test data with flexible column mapping
- Added REPOSITORY_LINK.txt for submission
</commit_message>
<xml_diff>
--- a/test-data/testcases.xlsx
+++ b/test-data/testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thisara/My disk/3y works/ITPM/IT23616356/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F87F190-CE78-0F47-AE25-F5E9DB8D896E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7CC6FD-E6F5-3E4C-BB6C-1B9106BA306E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="280">
   <si>
     <t>TC ID</t>
   </si>
@@ -58,9 +58,6 @@
     <t>M</t>
   </si>
   <si>
-    <t>Accurate Sinhala translation appears; meaning and punctuation preserved; Sinhala characters present.</t>
-  </si>
-  <si>
     <t>Not executed</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
     <t>S</t>
   </si>
   <si>
-    <t>Accurate Sinhala translation appears; sentence ends with full stop; Sinhala characters present.</t>
-  </si>
-  <si>
     <t>Simple declarative sentence; punctuation.</t>
   </si>
   <si>
@@ -94,9 +88,6 @@
     <t>Question about time</t>
   </si>
   <si>
-    <t>Accurate Sinhala translation appears; question form preserved; Sinhala characters present.</t>
-  </si>
-  <si>
     <t>Question structure; interrogative.</t>
   </si>
   <si>
@@ -109,9 +100,6 @@
     <t>Request/Polite</t>
   </si>
   <si>
-    <t>Accurate Sinhala translation appears; polite request meaning kept.</t>
-  </si>
-  <si>
     <t>Polite tone; request verb.</t>
   </si>
   <si>
@@ -124,9 +112,6 @@
     <t>Negation</t>
   </si>
   <si>
-    <t>Accurate Sinhala translation appears; negation preserved.</t>
-  </si>
-  <si>
     <t>Negative form should remain negative.</t>
   </si>
   <si>
@@ -139,9 +124,6 @@
     <t>Future plan</t>
   </si>
   <si>
-    <t>Accurate Sinhala translation appears; future intent kept.</t>
-  </si>
-  <si>
     <t>Future tense.</t>
   </si>
   <si>
@@ -154,9 +136,6 @@
     <t>Past tense</t>
   </si>
   <si>
-    <t>Accurate Sinhala translation appears; past meaning preserved.</t>
-  </si>
-  <si>
     <t>Past action.</t>
   </si>
   <si>
@@ -169,9 +148,6 @@
     <t>Numbers in sentence</t>
   </si>
   <si>
-    <t>Accurate Sinhala translation appears; number meaning preserved; Sinhala present.</t>
-  </si>
-  <si>
     <t>Numbers handling.</t>
   </si>
   <si>
@@ -184,9 +160,6 @@
     <t>Date format</t>
   </si>
   <si>
-    <t>Accurate Sinhala translation appears; date retained; Sinhala present.</t>
-  </si>
-  <si>
     <t>Date + statement.</t>
   </si>
   <si>
@@ -202,9 +175,6 @@
     <t>eka Rs. 1500k wage.</t>
   </si>
   <si>
-    <t>Accurate Sinhala translation appears; currency/number retained; Sinhala present.</t>
-  </si>
-  <si>
     <t>Currency formatting.</t>
   </si>
   <si>
@@ -217,9 +187,6 @@
     <t>Emphasis / exclamation</t>
   </si>
   <si>
-    <t>Accurate Sinhala translation appears; exclamation preserved; Sinhala present.</t>
-  </si>
-  <si>
     <t>Exclamation and interjection.</t>
   </si>
   <si>
@@ -232,9 +199,6 @@
     <t>Comma-separated list</t>
   </si>
   <si>
-    <t>Accurate Sinhala translation appears; list meaning preserved; Sinhala present.</t>
-  </si>
-  <si>
     <t>List punctuation.</t>
   </si>
   <si>
@@ -247,9 +211,6 @@
     <t>Quotation marks</t>
   </si>
   <si>
-    <t>Accurate Sinhala translation appears; quotes preserved or meaning maintained; Sinhala present.</t>
-  </si>
-  <si>
     <t>Quotes handling.</t>
   </si>
   <si>
@@ -262,9 +223,6 @@
     <t>Mixed case</t>
   </si>
   <si>
-    <t>Accurate Sinhala translation appears; case-insensitive input handled.</t>
-  </si>
-  <si>
     <t>Case-insensitive behavior.</t>
   </si>
   <si>
@@ -277,9 +235,6 @@
     <t>Extra spaces</t>
   </si>
   <si>
-    <t>Accurate Sinhala translation appears; extra spaces tolerated; Sinhala present.</t>
-  </si>
-  <si>
     <t>Whitespace robustness.</t>
   </si>
   <si>
@@ -292,12 +247,6 @@
     <t>Spelling variation</t>
   </si>
   <si>
-    <t>mama oyata adareyi</t>
-  </si>
-  <si>
-    <t>Accurate Sinhala translation appears; minor spelling variations tolerated; Sinhala present.</t>
-  </si>
-  <si>
     <t>Common variation handling.</t>
   </si>
   <si>
@@ -310,9 +259,6 @@
     <t>Long paragraph</t>
   </si>
   <si>
-    <t>Accurate Sinhala translation appears for whole paragraph; Sinhala present.</t>
-  </si>
-  <si>
     <t>Multi-sentence paragraph.</t>
   </si>
   <si>
@@ -325,9 +271,6 @@
     <t>Technical word kept</t>
   </si>
   <si>
-    <t>Sinhala translation appears; 'VS Code' preserved as-is; Sinhala present.</t>
-  </si>
-  <si>
     <t>Proper noun retention.</t>
   </si>
   <si>
@@ -340,9 +283,6 @@
     <t>Place names</t>
   </si>
   <si>
-    <t>Sinhala translation appears; place name handled; Sinhala present.</t>
-  </si>
-  <si>
     <t>Named entity handling.</t>
   </si>
   <si>
@@ -355,9 +295,6 @@
     <t>Phone number</t>
   </si>
   <si>
-    <t>Sinhala translation appears; phone number preserved; Sinhala present.</t>
-  </si>
-  <si>
     <t>Phone number handling.</t>
   </si>
   <si>
@@ -370,9 +307,6 @@
     <t>Emoji allowed</t>
   </si>
   <si>
-    <t>Sinhala translation appears; emoji does not break output; Sinhala present.</t>
-  </si>
-  <si>
     <t>Emoji robustness.</t>
   </si>
   <si>
@@ -388,9 +322,6 @@
     <t>mama online/offline mode balannam.</t>
   </si>
   <si>
-    <t>Sinhala translation appears; special chars handled; Sinhala present.</t>
-  </si>
-  <si>
     <t>Special chars in words.</t>
   </si>
   <si>
@@ -403,9 +334,6 @@
     <t>Short single word</t>
   </si>
   <si>
-    <t>Sinhala output appears (word conversion) or meaningful Sinhala equivalent; Sinhala present.</t>
-  </si>
-  <si>
     <t>Single-word conversion.</t>
   </si>
   <si>
@@ -421,9 +349,6 @@
     <t>L</t>
   </si>
   <si>
-    <t>Sinhala translation appears; app remains responsive; Sinhala present.</t>
-  </si>
-  <si>
     <t>Stress longer input while still valid.</t>
   </si>
   <si>
@@ -436,9 +361,6 @@
     <t>Conditional sentence</t>
   </si>
   <si>
-    <t>Accurate Sinhala translation appears; conditional meaning preserved; Sinhala present.</t>
-  </si>
-  <si>
     <t>Conditional structure handling.</t>
   </si>
   <si>
@@ -802,9 +724,6 @@
     <t>eya kivvee "mama enava" kiyala.</t>
   </si>
   <si>
-    <t>MaMa oYaTa aaDhAreyi.</t>
-  </si>
-  <si>
     <t>mama   oyaata    aadhareyi</t>
   </si>
   <si>
@@ -814,15 +733,9 @@
     <t>mama VS Code install kalaa.</t>
   </si>
   <si>
-    <t>mama colombo yanna hadhanava.</t>
-  </si>
-  <si>
     <t>aadharee</t>
   </si>
   <si>
-    <t>mama meeka test karanne input ekak venas venas vachana godak dhala system eka hadhanna puluwandha kiyala balanna. meka length eka vaedi Cheedhayak</t>
-  </si>
-  <si>
     <t>oya enavanam api yamu.</t>
   </si>
   <si>
@@ -839,6 +752,114 @@
   </si>
   <si>
     <t>suBha udhaeesanak! oyaa hodhin needha?</t>
+  </si>
+  <si>
+    <t>සුභ උදෑසනක්! ඔයා හොදින් නේද?</t>
+  </si>
+  <si>
+    <t>මම අද ගෙදර යනවා.</t>
+  </si>
+  <si>
+    <t>ඔය කවදද එන්නේ?</t>
+  </si>
+  <si>
+    <t>කරුණාකරලා මට help කරන්න.</t>
+  </si>
+  <si>
+    <t>මම ඒක කරන්නේ නෑ</t>
+  </si>
+  <si>
+    <t>හෙට අපි ගිහින් බලමු</t>
+  </si>
+  <si>
+    <t>මට කලින් කියල දුන්නා</t>
+  </si>
+  <si>
+    <t>මම items 3ක් ගත්තා</t>
+  </si>
+  <si>
+    <t>2026-01-30 ද මට exam තියෙනව.</t>
+  </si>
+  <si>
+    <t>එක Rs. 1500ක් wage.</t>
+  </si>
+  <si>
+    <t>wow! හරි ලස්සනයි!</t>
+  </si>
+  <si>
+    <t>මට tea, coffee, සහ juice ඕන.</t>
+  </si>
+  <si>
+    <t>එය කිව්වේ "මම එනව" කියල.</t>
+  </si>
+  <si>
+    <t>මම ඔයාට ආදරෙ​යි</t>
+  </si>
+  <si>
+    <t>MaMa oYa​aTa aaDhAreyi.</t>
+  </si>
+  <si>
+    <t>මම ඔYඅ​අඨ ආධරෙයි.</t>
+  </si>
+  <si>
+    <t>මම   ඔයාට    ආදරෙයි</t>
+  </si>
+  <si>
+    <t>mama oyaata aadhareyi</t>
+  </si>
+  <si>
+    <t>මම ඔයාට ආදරෙයි</t>
+  </si>
+  <si>
+    <t>මම අද ගෙදර යනවා. පස්සෙ මම බත් කනව. ඒට පස්සෙ මම වැඩ කරන්න plan කරනවා.</t>
+  </si>
+  <si>
+    <t>මම අද ගෙදර යනවා. පස්සෙ මම බත් කනව. ඒට පස්සෙ මම වැඩ කරන්න සැලසු​ම් කරනවා.</t>
+  </si>
+  <si>
+    <t>මම VS Code install කලා.</t>
+  </si>
+  <si>
+    <t>mama colombo yanna hadhanne.</t>
+  </si>
+  <si>
+    <t>මම colombo යන්න හදන්නෙ.</t>
+  </si>
+  <si>
+    <t>මම කොළ​ඹ යන්න හදන්නෙ.</t>
+  </si>
+  <si>
+    <t>මට call කරන්න 0714325672.</t>
+  </si>
+  <si>
+    <t>මට ඇමතුමක් කරන්න 0714325672.</t>
+  </si>
+  <si>
+    <t>මට හරි happy 😄</t>
+  </si>
+  <si>
+    <t>මට හරි සතුටුයි 😄</t>
+  </si>
+  <si>
+    <t>මම online/offline mode බලන්නම්.</t>
+  </si>
+  <si>
+    <t>මම මාර්ගග​ත/මාර්ගගත නොව​න වි​දි බලන්නම්.</t>
+  </si>
+  <si>
+    <t>ආදරේ</t>
+  </si>
+  <si>
+    <t>mama meeka test karanne input ekak venas venas vachana godak dhala system eka hadhanna puluvandha kiyala balanna. meka length eka vaedi Cheedhayak</t>
+  </si>
+  <si>
+    <t>මම මේක test කරන්නේ input එකක් වෙනස් වෙනස් වචන ගොඩක් දල system එක හදන්න පුලුවන්ද කියල බලන්න. මෙක length එක වැඩි ඡේදයක්</t>
+  </si>
+  <si>
+    <t>මම මේක පරීක්​ෂා කරන්නේ ආදාන වෙනස් වෙනස් වචන ගොඩක් දල පද්ධති​ය හදන්න පුලුවන්ද කියල බලන්න. මෙක දි​ග වැඩි ඡේදයක්</t>
+  </si>
+  <si>
+    <t>ඔය එනවනම් අපි යමු.</t>
   </si>
 </sst>
 </file>
@@ -1232,8 +1253,8 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1289,1206 +1310,1256 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>272</v>
+        <v>243</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2"/>
+        <v>244</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>244</v>
+      </c>
       <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>251</v>
+        <v>225</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="2"/>
+        <v>247</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>247</v>
+      </c>
       <c r="G5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>252</v>
+        <v>226</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="2"/>
+        <v>248</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>248</v>
+      </c>
       <c r="G6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>253</v>
+        <v>227</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="2"/>
+        <v>249</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>249</v>
+      </c>
       <c r="G7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>254</v>
+        <v>228</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="2"/>
+        <v>250</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>250</v>
+      </c>
       <c r="G8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>255</v>
+        <v>229</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="2"/>
+        <v>251</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>251</v>
+      </c>
       <c r="G9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="2"/>
+        <v>252</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>252</v>
+      </c>
       <c r="G10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="2"/>
+        <v>253</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="G11" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="2"/>
+        <v>254</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>254</v>
+      </c>
       <c r="G12" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>258</v>
+        <v>232</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" s="2"/>
+        <v>255</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>255</v>
+      </c>
       <c r="G13" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="2"/>
+        <v>256</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>256</v>
+      </c>
       <c r="G14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" s="2"/>
+        <v>257</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>259</v>
+      </c>
       <c r="G15" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>261</v>
+        <v>234</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F16" s="2"/>
+        <v>257</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>260</v>
+      </c>
       <c r="G16" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>90</v>
+        <v>261</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F17" s="2"/>
+        <v>262</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>262</v>
+      </c>
       <c r="G17" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>262</v>
+        <v>235</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F18" s="2"/>
+        <v>264</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>263</v>
+      </c>
       <c r="G18" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>263</v>
+        <v>236</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F19" s="2"/>
+        <v>265</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>265</v>
+      </c>
       <c r="G19" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F20" s="2"/>
+        <v>268</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>267</v>
+      </c>
       <c r="G20" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>247</v>
+        <v>221</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F21" s="2"/>
+        <v>270</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>269</v>
+      </c>
       <c r="G21" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>248</v>
+        <v>222</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F22" s="2"/>
+        <v>272</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>271</v>
+      </c>
       <c r="G22" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F23" s="2"/>
+        <v>274</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>273</v>
+      </c>
       <c r="G23" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>265</v>
+        <v>237</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F24" s="2"/>
+        <v>275</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>275</v>
+      </c>
       <c r="G24" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F25" s="2"/>
+        <v>278</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>277</v>
+      </c>
       <c r="G25" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>267</v>
+        <v>238</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F26" s="2"/>
+        <v>279</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>279</v>
+      </c>
       <c r="G26" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>160</v>
+        <v>134</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>169</v>
+        <v>143</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>170</v>
+        <v>144</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>171</v>
+        <v>145</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>175</v>
+        <v>149</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>176</v>
+        <v>150</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>177</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>178</v>
+        <v>152</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>268</v>
+        <v>239</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>180</v>
+        <v>154</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>182</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>183</v>
+        <v>157</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>185</v>
+        <v>159</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>186</v>
+        <v>160</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>182</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>189</v>
+        <v>163</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>269</v>
+        <v>240</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>190</v>
+        <v>164</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>191</v>
+        <v>165</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>193</v>
+        <v>167</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>196</v>
+        <v>170</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>270</v>
+        <v>241</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>177</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>202</v>
+        <v>176</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>203</v>
+        <v>177</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>204</v>
+        <v>178</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>205</v>
+        <v>179</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>207</v>
+        <v>181</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>208</v>
+        <v>182</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>209</v>
+        <v>183</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>210</v>
+        <v>184</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>211</v>
+        <v>185</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>212</v>
+        <v>186</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>213</v>
+        <v>187</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>214</v>
+        <v>188</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>215</v>
+        <v>189</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>216</v>
+        <v>190</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>217</v>
+        <v>191</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>218</v>
+        <v>192</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>219</v>
+        <v>193</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>220</v>
+        <v>194</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>221</v>
+        <v>195</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>222</v>
+        <v>196</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>223</v>
+        <v>197</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>224</v>
+        <v>198</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>225</v>
+        <v>199</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>271</v>
+        <v>242</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>226</v>
+        <v>200</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>227</v>
+        <v>201</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>228</v>
+        <v>202</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>229</v>
+        <v>203</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>230</v>
+        <v>204</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>231</v>
+        <v>205</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>232</v>
+        <v>206</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>233</v>
+        <v>207</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>234</v>
+        <v>208</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>235</v>
+        <v>209</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>236</v>
+        <v>210</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>237</v>
+        <v>211</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>238</v>
+        <v>212</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>239</v>
+        <v>213</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>240</v>
+        <v>214</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>241</v>
+        <v>215</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>246</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -2496,5 +2567,6 @@
     <hyperlink ref="D36" r:id="rId1" xr:uid="{68D28A0D-1646-C545-BC86-60F013B3FB7A}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>